<commit_message>
edited all expression sheet test files to include species name and taxon id
</commit_message>
<xml_diff>
--- a/test-files/expression-data-test-sheets/expression_sheet_empty_column.xlsx
+++ b/test-files/expression-data-test-sheets/expression_sheet_empty_column.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexi\OneDrive\GRNsight\test-files\expression-data-test-sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FSloaner\Ona\GRNsight\GRNsight\test-files\expression-data-test-sheets\To Do\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{37AC693B-6E5B-45E0-85D9-767B3D71F53D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{E15C0C3E-6A1B-406B-B039-5190B9870242}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="1000" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="wt_log2_expression" sheetId="6" r:id="rId1"/>
     <sheet name="network" sheetId="2" r:id="rId2"/>
     <sheet name="network_weights" sheetId="3" r:id="rId3"/>
+    <sheet name="optimization_parameters" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>ACE2</t>
   </si>
@@ -42,13 +42,82 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>optimization_parameter</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>kk_max</t>
+  </si>
+  <si>
+    <t>MaxIter</t>
+  </si>
+  <si>
+    <t>TolFun</t>
+  </si>
+  <si>
+    <t>MaxFunEval</t>
+  </si>
+  <si>
+    <t>TolX</t>
+  </si>
+  <si>
+    <t>production_function</t>
+  </si>
+  <si>
+    <t>Sigmoid</t>
+  </si>
+  <si>
+    <t>L_curve</t>
+  </si>
+  <si>
+    <t>estimate_params</t>
+  </si>
+  <si>
+    <t>make_graphs</t>
+  </si>
+  <si>
+    <t>fix_P</t>
+  </si>
+  <si>
+    <t>fix_b</t>
+  </si>
+  <si>
+    <t>expression_timepoints</t>
+  </si>
+  <si>
+    <t>Strain</t>
+  </si>
+  <si>
+    <t>wt</t>
+  </si>
+  <si>
+    <t>dgln3</t>
+  </si>
+  <si>
+    <t>simulation_timepoints</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>Saccharomyces cerevisiae</t>
+  </si>
+  <si>
+    <t>taxon_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -88,6 +157,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -106,7 +188,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="348">
+  <cellStyleXfs count="349">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -455,13 +537,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="348" applyFont="1"/>
+    <xf numFmtId="11" fontId="7" fillId="0" borderId="0" xfId="348" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="348"/>
   </cellXfs>
-  <cellStyles count="348">
+  <cellStyles count="349">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -809,7 +895,8 @@
     <cellStyle name="Hyperlink" xfId="344" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="346" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="277" xr:uid="{00000000-0005-0000-0000-00005B010000}"/>
+    <cellStyle name="Normal 2" xfId="348"/>
+    <cellStyle name="Normal 3" xfId="277"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1145,10 +1232,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1279,7 +1366,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1359,7 +1446,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1436,4 +1523,187 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5" style="3" customWidth="1"/>
+    <col min="2" max="1025" width="10.875" style="3" customWidth="1"/>
+    <col min="1026" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="4">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="3">
+        <v>15</v>
+      </c>
+      <c r="C14" s="3">
+        <v>30</v>
+      </c>
+      <c r="D14" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>5</v>
+      </c>
+      <c r="D16" s="3">
+        <v>10</v>
+      </c>
+      <c r="E16" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="3">
+        <v>559292</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
 </file>
</xml_diff>